<commit_message>
Update master data and optimization output with fixes
Changes:
1. Master_Data_Updated_Nov_Dec.xlsx:
   - Fixed BVCAD → KVCAD resource name typos in Part Master
   - 17 typos fixed affecting 39 parts (UBC-035, KBS-015, etc.)

2. production_plan_COMPREHENSIVE_test.xlsx:
   - Optimization output with buffer=2 fix
   - 100% fulfillment achieved (was 99.4%)
   - 0 units unmet (was 21 units)
   - All 303 orders fulfilled

3. fix_resource_names.py:
   - Script to fix BVCAD → KVCAD typos in Part Master
   - Automated resource name correction
</commit_message>
<xml_diff>
--- a/Master_Data_Updated_Nov_Dec.xlsx
+++ b/Master_Data_Updated_Nov_Dec.xlsx
@@ -11732,6 +11732,9 @@
           <t>KVCAD30MC001</t>
         </is>
       </c>
+      <c r="H2" t="n">
+        <v/>
+      </c>
       <c r="I2" t="n">
         <v>240</v>
       </c>
@@ -11776,6 +11779,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U2" t="n">
+        <v/>
+      </c>
+      <c r="V2" t="n">
+        <v/>
+      </c>
+      <c r="W2" t="n">
+        <v/>
+      </c>
       <c r="X2" t="n">
         <v>2</v>
       </c>
@@ -11867,6 +11879,12 @@
           <t>KVCAD30MC001</t>
         </is>
       </c>
+      <c r="G3" t="n">
+        <v/>
+      </c>
+      <c r="H3" t="n">
+        <v/>
+      </c>
       <c r="I3" t="n">
         <v>240</v>
       </c>
@@ -12170,6 +12188,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H5" t="n">
+        <v/>
+      </c>
       <c r="I5" t="n">
         <v>60</v>
       </c>
@@ -12319,6 +12340,9 @@
           <t>KVCAD30MC001</t>
         </is>
       </c>
+      <c r="H6" t="n">
+        <v/>
+      </c>
       <c r="I6" t="n">
         <v>240</v>
       </c>
@@ -12363,6 +12387,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U6" t="n">
+        <v/>
+      </c>
+      <c r="V6" t="n">
+        <v/>
+      </c>
+      <c r="W6" t="n">
+        <v/>
+      </c>
       <c r="X6" t="n">
         <v>2</v>
       </c>
@@ -12459,6 +12492,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H7" t="n">
+        <v/>
+      </c>
       <c r="I7" t="n">
         <v>40</v>
       </c>
@@ -12608,6 +12644,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H8" t="n">
+        <v/>
+      </c>
       <c r="I8" t="n">
         <v>40</v>
       </c>
@@ -12757,6 +12796,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H9" t="n">
+        <v/>
+      </c>
       <c r="I9" t="n">
         <v>40</v>
       </c>
@@ -12901,6 +12943,12 @@
           <t>MC1CKT-001</t>
         </is>
       </c>
+      <c r="G10" t="n">
+        <v/>
+      </c>
+      <c r="H10" t="n">
+        <v/>
+      </c>
       <c r="I10" t="n">
         <v>10</v>
       </c>
@@ -12935,6 +12983,21 @@
           <t>SP1CKT-001</t>
         </is>
       </c>
+      <c r="S10" t="n">
+        <v/>
+      </c>
+      <c r="T10" t="n">
+        <v/>
+      </c>
+      <c r="U10" t="n">
+        <v/>
+      </c>
+      <c r="V10" t="n">
+        <v/>
+      </c>
+      <c r="W10" t="n">
+        <v/>
+      </c>
       <c r="X10" t="n">
         <v>2</v>
       </c>
@@ -13022,7 +13085,7 @@
         <v>2</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -13381,6 +13444,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T13" t="n">
+        <v/>
+      </c>
+      <c r="U13" t="n">
+        <v/>
+      </c>
+      <c r="V13" t="n">
+        <v/>
+      </c>
+      <c r="W13" t="n">
+        <v/>
+      </c>
       <c r="X13" t="n">
         <v>2</v>
       </c>
@@ -13398,6 +13473,9 @@
       </c>
       <c r="AC13" t="n">
         <v>0</v>
+      </c>
+      <c r="AD13" t="n">
+        <v/>
       </c>
       <c r="AE13" t="n">
         <v>0</v>
@@ -13467,6 +13545,12 @@
           <t>MC1-DGC-004</t>
         </is>
       </c>
+      <c r="G14" t="n">
+        <v/>
+      </c>
+      <c r="H14" t="n">
+        <v/>
+      </c>
       <c r="I14" t="n">
         <v>90</v>
       </c>
@@ -13506,6 +13590,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T14" t="n">
+        <v/>
+      </c>
+      <c r="U14" t="n">
+        <v/>
+      </c>
+      <c r="V14" t="n">
+        <v/>
+      </c>
+      <c r="W14" t="n">
+        <v/>
+      </c>
       <c r="X14" t="n">
         <v>2</v>
       </c>
@@ -13523,6 +13619,9 @@
       </c>
       <c r="AC14" t="n">
         <v>0</v>
+      </c>
+      <c r="AD14" t="n">
+        <v/>
       </c>
       <c r="AE14" t="n">
         <v>0</v>
@@ -13592,6 +13691,12 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="G15" t="n">
+        <v/>
+      </c>
+      <c r="H15" t="n">
+        <v/>
+      </c>
       <c r="I15" t="n">
         <v>130</v>
       </c>
@@ -13631,6 +13736,9 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T15" t="n">
+        <v/>
+      </c>
       <c r="U15" t="n">
         <v>7</v>
       </c>
@@ -13881,7 +13989,13 @@
         <v>2</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v/>
+      </c>
+      <c r="G17" t="n">
+        <v/>
+      </c>
+      <c r="H17" t="n">
+        <v/>
       </c>
       <c r="I17" t="n">
         <v>0</v>
@@ -13922,6 +14036,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T17" t="n">
+        <v/>
+      </c>
+      <c r="U17" t="n">
+        <v/>
+      </c>
+      <c r="V17" t="n">
+        <v/>
+      </c>
+      <c r="W17" t="n">
+        <v/>
+      </c>
       <c r="X17" t="n">
         <v>2</v>
       </c>
@@ -14009,7 +14135,7 @@
         <v>4</v>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -14165,6 +14291,12 @@
           <t>MC1-DGC-009</t>
         </is>
       </c>
+      <c r="G19" t="n">
+        <v/>
+      </c>
+      <c r="H19" t="n">
+        <v/>
+      </c>
       <c r="I19" t="n">
         <v>25</v>
       </c>
@@ -14204,6 +14336,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T19" t="n">
+        <v/>
+      </c>
+      <c r="U19" t="n">
+        <v/>
+      </c>
+      <c r="V19" t="n">
+        <v/>
+      </c>
+      <c r="W19" t="n">
+        <v/>
+      </c>
       <c r="X19" t="n">
         <v>2</v>
       </c>
@@ -14221,6 +14365,9 @@
       </c>
       <c r="AC19" t="n">
         <v>0</v>
+      </c>
+      <c r="AD19" t="n">
+        <v/>
       </c>
       <c r="AE19" t="n">
         <v>0</v>
@@ -14440,7 +14587,7 @@
         <v>5</v>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -14755,6 +14902,9 @@
           <t>KVCAD40MC001</t>
         </is>
       </c>
+      <c r="H23" t="n">
+        <v/>
+      </c>
       <c r="I23" t="n">
         <v>150</v>
       </c>
@@ -14799,6 +14949,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U23" t="n">
+        <v/>
+      </c>
+      <c r="V23" t="n">
+        <v/>
+      </c>
+      <c r="W23" t="n">
+        <v/>
+      </c>
       <c r="X23" t="n">
         <v>2</v>
       </c>
@@ -14895,6 +15054,9 @@
           <t>KVCAD40MC001</t>
         </is>
       </c>
+      <c r="H24" t="n">
+        <v/>
+      </c>
       <c r="I24" t="n">
         <v>50</v>
       </c>
@@ -14939,6 +15101,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U24" t="n">
+        <v/>
+      </c>
+      <c r="V24" t="n">
+        <v/>
+      </c>
+      <c r="W24" t="n">
+        <v/>
+      </c>
       <c r="X24" t="n">
         <v>2</v>
       </c>
@@ -14956,6 +15127,9 @@
       </c>
       <c r="AC24" t="n">
         <v>1</v>
+      </c>
+      <c r="AD24" t="n">
+        <v/>
       </c>
       <c r="AE24" t="n">
         <v>0</v>
@@ -15030,6 +15204,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H25" t="n">
+        <v/>
+      </c>
       <c r="I25" t="n">
         <v>90</v>
       </c>
@@ -15074,6 +15251,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U25" t="n">
+        <v/>
+      </c>
+      <c r="V25" t="n">
+        <v/>
+      </c>
+      <c r="W25" t="n">
+        <v/>
+      </c>
       <c r="X25" t="n">
         <v>2</v>
       </c>
@@ -15091,6 +15277,9 @@
       </c>
       <c r="AC25" t="n">
         <v>1</v>
+      </c>
+      <c r="AD25" t="n">
+        <v/>
       </c>
       <c r="AE25" t="n">
         <v>0</v>
@@ -15165,6 +15354,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H26" t="n">
+        <v/>
+      </c>
       <c r="I26" t="n">
         <v>150</v>
       </c>
@@ -15209,6 +15401,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U26" t="n">
+        <v/>
+      </c>
+      <c r="V26" t="n">
+        <v/>
+      </c>
+      <c r="W26" t="n">
+        <v/>
+      </c>
       <c r="X26" t="n">
         <v>2</v>
       </c>
@@ -15302,8 +15503,11 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>BVCAD30MC001</t>
-        </is>
+          <t>KVCAD30MC001</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
+        <v/>
       </c>
       <c r="I27" t="n">
         <v>150</v>
@@ -15349,6 +15553,15 @@
           <t>BVCALFPSP001</t>
         </is>
       </c>
+      <c r="U27" t="n">
+        <v/>
+      </c>
+      <c r="V27" t="n">
+        <v/>
+      </c>
+      <c r="W27" t="n">
+        <v/>
+      </c>
       <c r="X27" t="n">
         <v>2</v>
       </c>
@@ -15366,6 +15579,9 @@
       </c>
       <c r="AC27" t="n">
         <v>1</v>
+      </c>
+      <c r="AD27" t="n">
+        <v/>
       </c>
       <c r="AE27" t="n">
         <v>0</v>
@@ -15440,6 +15656,9 @@
           <t>KVCAD30MC001</t>
         </is>
       </c>
+      <c r="H28" t="n">
+        <v/>
+      </c>
       <c r="I28" t="n">
         <v>50</v>
       </c>
@@ -15479,6 +15698,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T28" t="n">
+        <v/>
+      </c>
+      <c r="U28" t="n">
+        <v/>
+      </c>
+      <c r="V28" t="n">
+        <v/>
+      </c>
+      <c r="W28" t="n">
+        <v/>
+      </c>
       <c r="X28" t="n">
         <v>2</v>
       </c>
@@ -15567,7 +15798,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>BVCAD30MC001</t>
+          <t>KVCAD30MC001</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -15721,12 +15952,12 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>BVCAD30MC001</t>
+          <t>KVCAD30MC001</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>BVCAD30MC001</t>
+          <t>KVCAD30MC001</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -15883,6 +16114,9 @@
           <t>BVCABM1MC001</t>
         </is>
       </c>
+      <c r="H31" t="n">
+        <v/>
+      </c>
       <c r="I31" t="n">
         <v>90</v>
       </c>
@@ -15927,6 +16161,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U31" t="n">
+        <v/>
+      </c>
+      <c r="V31" t="n">
+        <v/>
+      </c>
+      <c r="W31" t="n">
+        <v/>
+      </c>
       <c r="X31" t="n">
         <v>2</v>
       </c>
@@ -16072,6 +16315,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U32" t="n">
+        <v/>
+      </c>
+      <c r="V32" t="n">
+        <v/>
+      </c>
+      <c r="W32" t="n">
+        <v/>
+      </c>
       <c r="X32" t="n">
         <v>2</v>
       </c>
@@ -16217,6 +16469,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U33" t="n">
+        <v/>
+      </c>
+      <c r="V33" t="n">
+        <v/>
+      </c>
+      <c r="W33" t="n">
+        <v/>
+      </c>
       <c r="X33" t="n">
         <v>2</v>
       </c>
@@ -16362,6 +16623,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U34" t="n">
+        <v/>
+      </c>
+      <c r="V34" t="n">
+        <v/>
+      </c>
+      <c r="W34" t="n">
+        <v/>
+      </c>
       <c r="X34" t="n">
         <v>2</v>
       </c>
@@ -16507,6 +16777,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U35" t="n">
+        <v/>
+      </c>
+      <c r="V35" t="n">
+        <v/>
+      </c>
+      <c r="W35" t="n">
+        <v/>
+      </c>
       <c r="X35" t="n">
         <v>2</v>
       </c>
@@ -16603,6 +16882,9 @@
           <t>KVCABM2MC001</t>
         </is>
       </c>
+      <c r="H36" t="n">
+        <v/>
+      </c>
       <c r="I36" t="n">
         <v>45</v>
       </c>
@@ -16647,6 +16929,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U36" t="n">
+        <v/>
+      </c>
+      <c r="V36" t="n">
+        <v/>
+      </c>
+      <c r="W36" t="n">
+        <v/>
+      </c>
       <c r="X36" t="n">
         <v>2</v>
       </c>
@@ -16743,6 +17034,9 @@
           <t>KVCAD40MC001</t>
         </is>
       </c>
+      <c r="H37" t="n">
+        <v/>
+      </c>
       <c r="I37" t="n">
         <v>45</v>
       </c>
@@ -16787,6 +17081,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U37" t="n">
+        <v/>
+      </c>
+      <c r="V37" t="n">
+        <v/>
+      </c>
+      <c r="W37" t="n">
+        <v/>
+      </c>
       <c r="X37" t="n">
         <v>2</v>
       </c>
@@ -16883,6 +17186,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H38" t="n">
+        <v/>
+      </c>
       <c r="I38" t="n">
         <v>45</v>
       </c>
@@ -16927,6 +17233,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U38" t="n">
+        <v/>
+      </c>
+      <c r="V38" t="n">
+        <v/>
+      </c>
+      <c r="W38" t="n">
+        <v/>
+      </c>
       <c r="X38" t="n">
         <v>2</v>
       </c>
@@ -17023,6 +17338,9 @@
           <t>KVCAD40MC001</t>
         </is>
       </c>
+      <c r="H39" t="n">
+        <v/>
+      </c>
       <c r="I39" t="n">
         <v>90</v>
       </c>
@@ -17318,8 +17636,14 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>BVCAD30MC001</t>
-        </is>
+          <t>KVCAD30MC001</t>
+        </is>
+      </c>
+      <c r="G41" t="n">
+        <v/>
+      </c>
+      <c r="H41" t="n">
+        <v/>
       </c>
       <c r="I41" t="n">
         <v>40</v>
@@ -17360,6 +17684,9 @@
           <t>BVCALPPSP002</t>
         </is>
       </c>
+      <c r="T41" t="n">
+        <v/>
+      </c>
       <c r="U41" t="n">
         <v>7</v>
       </c>
@@ -17457,8 +17784,14 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>BVCAD30MC001</t>
-        </is>
+          <t>KVCAD30MC001</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
+        <v/>
+      </c>
+      <c r="H42" t="n">
+        <v/>
       </c>
       <c r="I42" t="n">
         <v>40</v>
@@ -17499,6 +17832,9 @@
           <t>BVCALPPSP002</t>
         </is>
       </c>
+      <c r="T42" t="n">
+        <v/>
+      </c>
       <c r="U42" t="n">
         <v>7</v>
       </c>
@@ -17604,6 +17940,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H43" t="n">
+        <v/>
+      </c>
       <c r="I43" t="n">
         <v>30</v>
       </c>
@@ -17753,6 +18092,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H44" t="n">
+        <v/>
+      </c>
       <c r="I44" t="n">
         <v>30</v>
       </c>
@@ -17902,6 +18244,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H45" t="n">
+        <v/>
+      </c>
       <c r="I45" t="n">
         <v>20</v>
       </c>
@@ -18051,6 +18396,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H46" t="n">
+        <v/>
+      </c>
       <c r="I46" t="n">
         <v>30</v>
       </c>
@@ -18200,6 +18548,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H47" t="n">
+        <v/>
+      </c>
       <c r="I47" t="n">
         <v>25</v>
       </c>
@@ -18349,6 +18700,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H48" t="n">
+        <v/>
+      </c>
       <c r="I48" t="n">
         <v>25</v>
       </c>
@@ -18498,6 +18852,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H49" t="n">
+        <v/>
+      </c>
       <c r="I49" t="n">
         <v>25</v>
       </c>
@@ -18537,6 +18894,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T49" t="n">
+        <v/>
+      </c>
+      <c r="U49" t="n">
+        <v/>
+      </c>
+      <c r="V49" t="n">
+        <v/>
+      </c>
+      <c r="W49" t="n">
+        <v/>
+      </c>
       <c r="X49" t="n">
         <v>2</v>
       </c>
@@ -18633,6 +19002,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H50" t="n">
+        <v/>
+      </c>
       <c r="I50" t="n">
         <v>30</v>
       </c>
@@ -18672,6 +19044,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T50" t="n">
+        <v/>
+      </c>
+      <c r="U50" t="n">
+        <v/>
+      </c>
+      <c r="V50" t="n">
+        <v/>
+      </c>
+      <c r="W50" t="n">
+        <v/>
+      </c>
       <c r="X50" t="n">
         <v>2</v>
       </c>
@@ -18689,6 +19073,9 @@
       </c>
       <c r="AC50" t="n">
         <v>1</v>
+      </c>
+      <c r="AD50" t="n">
+        <v/>
       </c>
       <c r="AE50" t="n">
         <v>0</v>
@@ -18763,6 +19150,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H51" t="n">
+        <v/>
+      </c>
       <c r="I51" t="n">
         <v>30</v>
       </c>
@@ -18802,6 +19192,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T51" t="n">
+        <v/>
+      </c>
+      <c r="U51" t="n">
+        <v/>
+      </c>
+      <c r="V51" t="n">
+        <v/>
+      </c>
+      <c r="W51" t="n">
+        <v/>
+      </c>
       <c r="X51" t="n">
         <v>2</v>
       </c>
@@ -18819,6 +19221,9 @@
       </c>
       <c r="AC51" t="n">
         <v>1</v>
+      </c>
+      <c r="AD51" t="n">
+        <v/>
       </c>
       <c r="AE51" t="n">
         <v>0</v>
@@ -18893,6 +19298,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H52" t="n">
+        <v/>
+      </c>
       <c r="I52" t="n">
         <v>20</v>
       </c>
@@ -19042,6 +19450,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H53" t="n">
+        <v/>
+      </c>
       <c r="I53" t="n">
         <v>35</v>
       </c>
@@ -19191,6 +19602,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H54" t="n">
+        <v/>
+      </c>
       <c r="I54" t="n">
         <v>35</v>
       </c>
@@ -19335,6 +19749,12 @@
           <t>KVCALHTMC001</t>
         </is>
       </c>
+      <c r="G55" t="n">
+        <v/>
+      </c>
+      <c r="H55" t="n">
+        <v/>
+      </c>
       <c r="I55" t="n">
         <v>25</v>
       </c>
@@ -19484,6 +19904,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H56" t="n">
+        <v/>
+      </c>
       <c r="I56" t="n">
         <v>40</v>
       </c>
@@ -19633,6 +20056,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H57" t="n">
+        <v/>
+      </c>
       <c r="I57" t="n">
         <v>30</v>
       </c>
@@ -19777,6 +20203,12 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="G58" t="n">
+        <v/>
+      </c>
+      <c r="H58" t="n">
+        <v/>
+      </c>
       <c r="I58" t="n">
         <v>90</v>
       </c>
@@ -19921,6 +20353,12 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="G59" t="n">
+        <v/>
+      </c>
+      <c r="H59" t="n">
+        <v/>
+      </c>
       <c r="I59" t="n">
         <v>40</v>
       </c>
@@ -20065,6 +20503,12 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="G60" t="n">
+        <v/>
+      </c>
+      <c r="H60" t="n">
+        <v/>
+      </c>
       <c r="I60" t="n">
         <v>150</v>
       </c>
@@ -20209,6 +20653,12 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="G61" t="n">
+        <v/>
+      </c>
+      <c r="H61" t="n">
+        <v/>
+      </c>
       <c r="I61" t="n">
         <v>40</v>
       </c>
@@ -20358,6 +20808,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H62" t="n">
+        <v/>
+      </c>
       <c r="I62" t="n">
         <v>30</v>
       </c>
@@ -20498,7 +20951,7 @@
         <v>1</v>
       </c>
       <c r="F63" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -20650,7 +21103,7 @@
         <v>1</v>
       </c>
       <c r="F64" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -20965,6 +21418,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H66" t="n">
+        <v/>
+      </c>
       <c r="I66" t="n">
         <v>40</v>
       </c>
@@ -21114,6 +21570,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H67" t="n">
+        <v/>
+      </c>
       <c r="I67" t="n">
         <v>40</v>
       </c>
@@ -21263,6 +21722,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H68" t="n">
+        <v/>
+      </c>
       <c r="I68" t="n">
         <v>40</v>
       </c>
@@ -21412,6 +21874,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H69" t="n">
+        <v/>
+      </c>
       <c r="I69" t="n">
         <v>40</v>
       </c>
@@ -21561,6 +22026,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H70" t="n">
+        <v/>
+      </c>
       <c r="I70" t="n">
         <v>40</v>
       </c>
@@ -21705,6 +22173,12 @@
           <t>MC1-MGB-001</t>
         </is>
       </c>
+      <c r="G71" t="n">
+        <v/>
+      </c>
+      <c r="H71" t="n">
+        <v/>
+      </c>
       <c r="I71" t="n">
         <v>30</v>
       </c>
@@ -21744,6 +22218,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T71" t="n">
+        <v/>
+      </c>
+      <c r="U71" t="n">
+        <v/>
+      </c>
+      <c r="V71" t="n">
+        <v/>
+      </c>
+      <c r="W71" t="n">
+        <v/>
+      </c>
       <c r="X71" t="n">
         <v>2</v>
       </c>
@@ -21840,6 +22326,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H72" t="n">
+        <v/>
+      </c>
       <c r="I72" t="n">
         <v>60</v>
       </c>
@@ -21980,7 +22469,7 @@
         <v>2</v>
       </c>
       <c r="F73" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -22132,7 +22621,7 @@
         <v>1</v>
       </c>
       <c r="F74" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -22288,6 +22777,12 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="G75" t="n">
+        <v/>
+      </c>
+      <c r="H75" t="n">
+        <v/>
+      </c>
       <c r="I75" t="n">
         <v>40</v>
       </c>
@@ -22437,6 +22932,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H76" t="n">
+        <v/>
+      </c>
       <c r="I76" t="n">
         <v>60</v>
       </c>
@@ -22476,6 +22974,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T76" t="n">
+        <v/>
+      </c>
+      <c r="U76" t="n">
+        <v/>
+      </c>
+      <c r="V76" t="n">
+        <v/>
+      </c>
+      <c r="W76" t="n">
+        <v/>
+      </c>
       <c r="X76" t="n">
         <v>2</v>
       </c>
@@ -22563,7 +23073,13 @@
         <v>6</v>
       </c>
       <c r="F77" t="n">
-        <v>0</v>
+        <v/>
+      </c>
+      <c r="G77" t="n">
+        <v/>
+      </c>
+      <c r="H77" t="n">
+        <v/>
       </c>
       <c r="I77" t="n">
         <v>0</v>
@@ -22604,6 +23120,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T77" t="n">
+        <v/>
+      </c>
+      <c r="U77" t="n">
+        <v/>
+      </c>
+      <c r="V77" t="n">
+        <v/>
+      </c>
+      <c r="W77" t="n">
+        <v/>
+      </c>
       <c r="X77" t="n">
         <v>2</v>
       </c>
@@ -22621,6 +23149,9 @@
       </c>
       <c r="AC77" t="n">
         <v>1</v>
+      </c>
+      <c r="AD77" t="n">
+        <v/>
       </c>
       <c r="AE77" t="n">
         <v>0</v>
@@ -22695,6 +23226,9 @@
           <t>KVCAD10MC001</t>
         </is>
       </c>
+      <c r="H78" t="n">
+        <v/>
+      </c>
       <c r="I78" t="n">
         <v>40</v>
       </c>
@@ -22734,6 +23268,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T78" t="n">
+        <v/>
+      </c>
+      <c r="U78" t="n">
+        <v/>
+      </c>
+      <c r="V78" t="n">
+        <v/>
+      </c>
+      <c r="W78" t="n">
+        <v/>
+      </c>
       <c r="X78" t="n">
         <v>2</v>
       </c>
@@ -22830,6 +23376,9 @@
           <t>KVCAD10MC001</t>
         </is>
       </c>
+      <c r="H79" t="n">
+        <v/>
+      </c>
       <c r="I79" t="n">
         <v>40</v>
       </c>
@@ -22869,6 +23418,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T79" t="n">
+        <v/>
+      </c>
+      <c r="U79" t="n">
+        <v/>
+      </c>
+      <c r="V79" t="n">
+        <v/>
+      </c>
+      <c r="W79" t="n">
+        <v/>
+      </c>
       <c r="X79" t="n">
         <v>2</v>
       </c>
@@ -23119,6 +23680,9 @@
           <t>KVCAD40MC001</t>
         </is>
       </c>
+      <c r="H81" t="n">
+        <v/>
+      </c>
       <c r="I81" t="n">
         <v>90</v>
       </c>
@@ -23163,6 +23727,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U81" t="n">
+        <v/>
+      </c>
+      <c r="V81" t="n">
+        <v/>
+      </c>
+      <c r="W81" t="n">
+        <v/>
+      </c>
       <c r="X81" t="n">
         <v>2</v>
       </c>
@@ -23259,6 +23832,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H82" t="n">
+        <v/>
+      </c>
       <c r="I82" t="n">
         <v>20</v>
       </c>
@@ -23399,7 +23975,7 @@
         <v>3</v>
       </c>
       <c r="F83" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="G83" t="inlineStr">
         <is>
@@ -23551,7 +24127,7 @@
         <v>5</v>
       </c>
       <c r="F84" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -23703,7 +24279,7 @@
         <v>6</v>
       </c>
       <c r="F85" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="G85" t="inlineStr">
         <is>
@@ -23859,6 +24435,12 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="G86" t="n">
+        <v/>
+      </c>
+      <c r="H86" t="n">
+        <v/>
+      </c>
       <c r="I86" t="n">
         <v>40</v>
       </c>
@@ -24003,6 +24585,12 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="G87" t="n">
+        <v/>
+      </c>
+      <c r="H87" t="n">
+        <v/>
+      </c>
       <c r="I87" t="n">
         <v>20</v>
       </c>
@@ -24152,6 +24740,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H88" t="n">
+        <v/>
+      </c>
       <c r="I88" t="n">
         <v>60</v>
       </c>
@@ -24301,6 +24892,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H89" t="n">
+        <v/>
+      </c>
       <c r="I89" t="n">
         <v>60</v>
       </c>
@@ -24345,6 +24939,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U89" t="n">
+        <v/>
+      </c>
+      <c r="V89" t="n">
+        <v/>
+      </c>
+      <c r="W89" t="n">
+        <v/>
+      </c>
       <c r="X89" t="n">
         <v>2</v>
       </c>
@@ -24441,6 +25044,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H90" t="n">
+        <v/>
+      </c>
       <c r="I90" t="n">
         <v>60</v>
       </c>
@@ -24590,6 +25196,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H91" t="n">
+        <v/>
+      </c>
       <c r="I91" t="n">
         <v>60</v>
       </c>
@@ -24739,6 +25348,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H92" t="n">
+        <v/>
+      </c>
       <c r="I92" t="n">
         <v>40</v>
       </c>
@@ -24883,6 +25495,12 @@
           <t>MC1-TAS-GN-015</t>
         </is>
       </c>
+      <c r="G93" t="n">
+        <v/>
+      </c>
+      <c r="H93" t="n">
+        <v/>
+      </c>
       <c r="I93" t="n">
         <v>30</v>
       </c>
@@ -24927,6 +25545,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U93" t="n">
+        <v/>
+      </c>
+      <c r="V93" t="n">
+        <v/>
+      </c>
+      <c r="W93" t="n">
+        <v/>
+      </c>
       <c r="X93" t="n">
         <v>2</v>
       </c>
@@ -24944,6 +25571,9 @@
       </c>
       <c r="AC93" t="n">
         <v>1</v>
+      </c>
+      <c r="AD93" t="n">
+        <v/>
       </c>
       <c r="AE93" t="n">
         <v>0</v>
@@ -25167,6 +25797,12 @@
           <t>MC1-TAS-GN-017</t>
         </is>
       </c>
+      <c r="G95" t="n">
+        <v/>
+      </c>
+      <c r="H95" t="n">
+        <v/>
+      </c>
       <c r="I95" t="n">
         <v>30</v>
       </c>
@@ -25211,6 +25847,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U95" t="n">
+        <v/>
+      </c>
+      <c r="V95" t="n">
+        <v/>
+      </c>
+      <c r="W95" t="n">
+        <v/>
+      </c>
       <c r="X95" t="n">
         <v>2</v>
       </c>
@@ -25228,6 +25873,9 @@
       </c>
       <c r="AC95" t="n">
         <v>1</v>
+      </c>
+      <c r="AD95" t="n">
+        <v/>
       </c>
       <c r="AE95" t="n">
         <v>0</v>
@@ -25293,7 +25941,13 @@
         <v>6</v>
       </c>
       <c r="F96" t="n">
-        <v>0</v>
+        <v/>
+      </c>
+      <c r="G96" t="n">
+        <v/>
+      </c>
+      <c r="H96" t="n">
+        <v/>
       </c>
       <c r="I96" t="n">
         <v>0</v>
@@ -25339,6 +25993,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U96" t="n">
+        <v/>
+      </c>
+      <c r="V96" t="n">
+        <v/>
+      </c>
+      <c r="W96" t="n">
+        <v/>
+      </c>
       <c r="X96" t="n">
         <v>2</v>
       </c>
@@ -25426,7 +26089,13 @@
         <v>4</v>
       </c>
       <c r="F97" t="n">
-        <v>0</v>
+        <v/>
+      </c>
+      <c r="G97" t="n">
+        <v/>
+      </c>
+      <c r="H97" t="n">
+        <v/>
       </c>
       <c r="I97" t="n">
         <v>0</v>
@@ -25472,6 +26141,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U97" t="n">
+        <v/>
+      </c>
+      <c r="V97" t="n">
+        <v/>
+      </c>
+      <c r="W97" t="n">
+        <v/>
+      </c>
       <c r="X97" t="n">
         <v>2</v>
       </c>
@@ -25489,6 +26167,9 @@
       </c>
       <c r="AC97" t="n">
         <v>1</v>
+      </c>
+      <c r="AD97" t="n">
+        <v/>
       </c>
       <c r="AE97" t="n">
         <v>0</v>
@@ -25558,6 +26239,12 @@
           <t>MC1-TAS-GN-020</t>
         </is>
       </c>
+      <c r="G98" t="n">
+        <v/>
+      </c>
+      <c r="H98" t="n">
+        <v/>
+      </c>
       <c r="I98" t="n">
         <v>30</v>
       </c>
@@ -25602,6 +26289,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U98" t="n">
+        <v/>
+      </c>
+      <c r="V98" t="n">
+        <v/>
+      </c>
+      <c r="W98" t="n">
+        <v/>
+      </c>
       <c r="X98" t="n">
         <v>2</v>
       </c>
@@ -25689,7 +26385,7 @@
         <v>4</v>
       </c>
       <c r="F99" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="G99" t="inlineStr">
         <is>
@@ -25845,6 +26541,12 @@
           <t>MC1-TAS-GN-022</t>
         </is>
       </c>
+      <c r="G100" t="n">
+        <v/>
+      </c>
+      <c r="H100" t="n">
+        <v/>
+      </c>
       <c r="I100" t="n">
         <v>40</v>
       </c>
@@ -25889,6 +26591,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U100" t="n">
+        <v/>
+      </c>
+      <c r="V100" t="n">
+        <v/>
+      </c>
+      <c r="W100" t="n">
+        <v/>
+      </c>
       <c r="X100" t="n">
         <v>2</v>
       </c>
@@ -25980,6 +26691,12 @@
           <t>MC1-TAS-GN-028</t>
         </is>
       </c>
+      <c r="G101" t="n">
+        <v/>
+      </c>
+      <c r="H101" t="n">
+        <v/>
+      </c>
       <c r="I101" t="n">
         <v>150</v>
       </c>
@@ -26024,6 +26741,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U101" t="n">
+        <v/>
+      </c>
+      <c r="V101" t="n">
+        <v/>
+      </c>
+      <c r="W101" t="n">
+        <v/>
+      </c>
       <c r="X101" t="n">
         <v>2</v>
       </c>
@@ -26041,6 +26767,9 @@
       </c>
       <c r="AC101" t="n">
         <v>1</v>
+      </c>
+      <c r="AD101" t="n">
+        <v/>
       </c>
       <c r="AE101" t="n">
         <v>0</v>
@@ -26106,7 +26835,7 @@
         <v>4</v>
       </c>
       <c r="F102" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="G102" t="inlineStr">
         <is>
@@ -26267,6 +26996,9 @@
           <t>KVCACNCMC001</t>
         </is>
       </c>
+      <c r="H103" t="n">
+        <v/>
+      </c>
       <c r="I103" t="n">
         <v>180</v>
       </c>
@@ -26306,6 +27038,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T103" t="n">
+        <v/>
+      </c>
+      <c r="U103" t="n">
+        <v/>
+      </c>
+      <c r="V103" t="n">
+        <v/>
+      </c>
+      <c r="W103" t="n">
+        <v/>
+      </c>
       <c r="X103" t="n">
         <v>2</v>
       </c>
@@ -26397,6 +27141,12 @@
           <t>MC1-UBC-012</t>
         </is>
       </c>
+      <c r="G104" t="n">
+        <v/>
+      </c>
+      <c r="H104" t="n">
+        <v/>
+      </c>
       <c r="I104" t="n">
         <v>30</v>
       </c>
@@ -26436,6 +27186,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T104" t="n">
+        <v/>
+      </c>
+      <c r="U104" t="n">
+        <v/>
+      </c>
+      <c r="V104" t="n">
+        <v/>
+      </c>
+      <c r="W104" t="n">
+        <v/>
+      </c>
       <c r="X104" t="n">
         <v>2</v>
       </c>
@@ -26453,6 +27215,9 @@
       </c>
       <c r="AC104" t="n">
         <v>0</v>
+      </c>
+      <c r="AD104" t="n">
+        <v/>
       </c>
       <c r="AE104" t="n">
         <v>0</v>
@@ -26522,6 +27287,12 @@
           <t>MC1-UBC-013</t>
         </is>
       </c>
+      <c r="G105" t="n">
+        <v/>
+      </c>
+      <c r="H105" t="n">
+        <v/>
+      </c>
       <c r="I105" t="n">
         <v>30</v>
       </c>
@@ -26561,6 +27332,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T105" t="n">
+        <v/>
+      </c>
+      <c r="U105" t="n">
+        <v/>
+      </c>
+      <c r="V105" t="n">
+        <v/>
+      </c>
+      <c r="W105" t="n">
+        <v/>
+      </c>
       <c r="X105" t="n">
         <v>2</v>
       </c>
@@ -26578,6 +27361,9 @@
       </c>
       <c r="AC105" t="n">
         <v>0</v>
+      </c>
+      <c r="AD105" t="n">
+        <v/>
       </c>
       <c r="AE105" t="n">
         <v>0</v>
@@ -26801,6 +27587,12 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="G107" t="n">
+        <v/>
+      </c>
+      <c r="H107" t="n">
+        <v/>
+      </c>
       <c r="I107" t="n">
         <v>20</v>
       </c>
@@ -26945,6 +27737,12 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="G108" t="n">
+        <v/>
+      </c>
+      <c r="H108" t="n">
+        <v/>
+      </c>
       <c r="I108" t="n">
         <v>20</v>
       </c>
@@ -27085,7 +27883,7 @@
         <v>1</v>
       </c>
       <c r="F109" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="G109" t="inlineStr">
         <is>
@@ -27246,6 +28044,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H110" t="n">
+        <v/>
+      </c>
       <c r="I110" t="n">
         <v>80</v>
       </c>
@@ -27395,6 +28196,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H111" t="n">
+        <v/>
+      </c>
       <c r="I111" t="n">
         <v>60</v>
       </c>
@@ -27434,6 +28238,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T111" t="n">
+        <v/>
+      </c>
+      <c r="U111" t="n">
+        <v/>
+      </c>
+      <c r="V111" t="n">
+        <v/>
+      </c>
+      <c r="W111" t="n">
+        <v/>
+      </c>
       <c r="X111" t="n">
         <v>2</v>
       </c>
@@ -27451,6 +28267,9 @@
       </c>
       <c r="AC111" t="n">
         <v>1</v>
+      </c>
+      <c r="AD111" t="n">
+        <v/>
       </c>
       <c r="AE111" t="n">
         <v>0</v>
@@ -27525,6 +28344,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H112" t="n">
+        <v/>
+      </c>
       <c r="I112" t="n">
         <v>60</v>
       </c>
@@ -27564,6 +28386,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T112" t="n">
+        <v/>
+      </c>
+      <c r="U112" t="n">
+        <v/>
+      </c>
+      <c r="V112" t="n">
+        <v/>
+      </c>
+      <c r="W112" t="n">
+        <v/>
+      </c>
       <c r="X112" t="n">
         <v>2</v>
       </c>
@@ -27660,6 +28494,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H113" t="n">
+        <v/>
+      </c>
       <c r="I113" t="n">
         <v>180</v>
       </c>
@@ -27699,6 +28536,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T113" t="n">
+        <v/>
+      </c>
+      <c r="U113" t="n">
+        <v/>
+      </c>
+      <c r="V113" t="n">
+        <v/>
+      </c>
+      <c r="W113" t="n">
+        <v/>
+      </c>
       <c r="X113" t="n">
         <v>2</v>
       </c>
@@ -27795,6 +28644,9 @@
           <t>KVCAD30MC001</t>
         </is>
       </c>
+      <c r="H114" t="n">
+        <v/>
+      </c>
       <c r="I114" t="n">
         <v>90</v>
       </c>
@@ -27834,6 +28686,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T114" t="n">
+        <v/>
+      </c>
+      <c r="U114" t="n">
+        <v/>
+      </c>
+      <c r="V114" t="n">
+        <v/>
+      </c>
+      <c r="W114" t="n">
+        <v/>
+      </c>
       <c r="X114" t="n">
         <v>2</v>
       </c>
@@ -27922,13 +28786,16 @@
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>BVCAD30MC001</t>
+          <t>KVCAD30MC001</t>
         </is>
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>BVCAD40MC001</t>
-        </is>
+          <t>KVCAD40MC001</t>
+        </is>
+      </c>
+      <c r="H115" t="n">
+        <v/>
       </c>
       <c r="I115" t="n">
         <v>90</v>
@@ -28079,6 +28946,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H116" t="n">
+        <v/>
+      </c>
       <c r="I116" t="n">
         <v>90</v>
       </c>
@@ -28118,6 +28988,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T116" t="n">
+        <v/>
+      </c>
+      <c r="U116" t="n">
+        <v/>
+      </c>
+      <c r="V116" t="n">
+        <v/>
+      </c>
+      <c r="W116" t="n">
+        <v/>
+      </c>
       <c r="X116" t="n">
         <v>2</v>
       </c>
@@ -28214,6 +29096,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H117" t="n">
+        <v/>
+      </c>
       <c r="I117" t="n">
         <v>90</v>
       </c>
@@ -28253,6 +29138,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T117" t="n">
+        <v/>
+      </c>
+      <c r="U117" t="n">
+        <v/>
+      </c>
+      <c r="V117" t="n">
+        <v/>
+      </c>
+      <c r="W117" t="n">
+        <v/>
+      </c>
       <c r="X117" t="n">
         <v>2</v>
       </c>
@@ -28349,6 +29246,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H118" t="n">
+        <v/>
+      </c>
       <c r="I118" t="n">
         <v>90</v>
       </c>
@@ -28388,6 +29288,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T118" t="n">
+        <v/>
+      </c>
+      <c r="U118" t="n">
+        <v/>
+      </c>
+      <c r="V118" t="n">
+        <v/>
+      </c>
+      <c r="W118" t="n">
+        <v/>
+      </c>
       <c r="X118" t="n">
         <v>2</v>
       </c>
@@ -28484,6 +29396,9 @@
           <t>KVCAD30MC001</t>
         </is>
       </c>
+      <c r="H119" t="n">
+        <v/>
+      </c>
       <c r="I119" t="n">
         <v>90</v>
       </c>
@@ -28523,6 +29438,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T119" t="n">
+        <v/>
+      </c>
+      <c r="U119" t="n">
+        <v/>
+      </c>
+      <c r="V119" t="n">
+        <v/>
+      </c>
+      <c r="W119" t="n">
+        <v/>
+      </c>
       <c r="X119" t="n">
         <v>2</v>
       </c>
@@ -28619,6 +29546,9 @@
           <t>KVCAD30MC001</t>
         </is>
       </c>
+      <c r="H120" t="n">
+        <v/>
+      </c>
       <c r="I120" t="n">
         <v>90</v>
       </c>
@@ -28658,6 +29588,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T120" t="n">
+        <v/>
+      </c>
+      <c r="U120" t="n">
+        <v/>
+      </c>
+      <c r="V120" t="n">
+        <v/>
+      </c>
+      <c r="W120" t="n">
+        <v/>
+      </c>
       <c r="X120" t="n">
         <v>2</v>
       </c>
@@ -28754,6 +29696,9 @@
           <t>KVCAD30MC001</t>
         </is>
       </c>
+      <c r="H121" t="n">
+        <v/>
+      </c>
       <c r="I121" t="n">
         <v>90</v>
       </c>
@@ -28793,6 +29738,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T121" t="n">
+        <v/>
+      </c>
+      <c r="U121" t="n">
+        <v/>
+      </c>
+      <c r="V121" t="n">
+        <v/>
+      </c>
+      <c r="W121" t="n">
+        <v/>
+      </c>
       <c r="X121" t="n">
         <v>2</v>
       </c>
@@ -28889,6 +29846,9 @@
           <t>KVCAD30MC001</t>
         </is>
       </c>
+      <c r="H122" t="n">
+        <v/>
+      </c>
       <c r="I122" t="n">
         <v>90</v>
       </c>
@@ -28928,6 +29888,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T122" t="n">
+        <v/>
+      </c>
+      <c r="U122" t="n">
+        <v/>
+      </c>
+      <c r="V122" t="n">
+        <v/>
+      </c>
+      <c r="W122" t="n">
+        <v/>
+      </c>
       <c r="X122" t="n">
         <v>2</v>
       </c>
@@ -29024,6 +29996,9 @@
           <t>KVCAD30MC001</t>
         </is>
       </c>
+      <c r="H123" t="n">
+        <v/>
+      </c>
       <c r="I123" t="n">
         <v>90</v>
       </c>
@@ -29063,6 +30038,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T123" t="n">
+        <v/>
+      </c>
+      <c r="U123" t="n">
+        <v/>
+      </c>
+      <c r="V123" t="n">
+        <v/>
+      </c>
+      <c r="W123" t="n">
+        <v/>
+      </c>
       <c r="X123" t="n">
         <v>2</v>
       </c>
@@ -29159,6 +30146,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H124" t="n">
+        <v/>
+      </c>
       <c r="I124" t="n">
         <v>90</v>
       </c>
@@ -29198,6 +30188,18 @@
           <t>BVCALPPSP002</t>
         </is>
       </c>
+      <c r="T124" t="n">
+        <v/>
+      </c>
+      <c r="U124" t="n">
+        <v/>
+      </c>
+      <c r="V124" t="n">
+        <v/>
+      </c>
+      <c r="W124" t="n">
+        <v/>
+      </c>
       <c r="X124" t="n">
         <v>2</v>
       </c>
@@ -29285,7 +30287,13 @@
         <v>2</v>
       </c>
       <c r="F125" t="n">
-        <v>0</v>
+        <v/>
+      </c>
+      <c r="G125" t="n">
+        <v/>
+      </c>
+      <c r="H125" t="n">
+        <v/>
       </c>
       <c r="I125" t="n">
         <v>0</v>
@@ -29326,6 +30334,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T125" t="n">
+        <v/>
+      </c>
+      <c r="U125" t="n">
+        <v/>
+      </c>
+      <c r="V125" t="n">
+        <v/>
+      </c>
+      <c r="W125" t="n">
+        <v/>
+      </c>
       <c r="X125" t="n">
         <v>2</v>
       </c>
@@ -29413,7 +30433,13 @@
         <v>2</v>
       </c>
       <c r="F126" t="n">
-        <v>0</v>
+        <v/>
+      </c>
+      <c r="G126" t="n">
+        <v/>
+      </c>
+      <c r="H126" t="n">
+        <v/>
       </c>
       <c r="I126" t="n">
         <v>0</v>
@@ -29454,6 +30480,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T126" t="n">
+        <v/>
+      </c>
+      <c r="U126" t="n">
+        <v/>
+      </c>
+      <c r="V126" t="n">
+        <v/>
+      </c>
+      <c r="W126" t="n">
+        <v/>
+      </c>
       <c r="X126" t="n">
         <v>2</v>
       </c>
@@ -29541,7 +30579,7 @@
         <v>3</v>
       </c>
       <c r="F127" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="G127" t="inlineStr">
         <is>
@@ -29693,7 +30731,7 @@
         <v>3</v>
       </c>
       <c r="F128" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="G128" t="inlineStr">
         <is>
@@ -29854,6 +30892,9 @@
           <t>KVCAD30MC001</t>
         </is>
       </c>
+      <c r="H129" t="n">
+        <v/>
+      </c>
       <c r="I129" t="n">
         <v>90</v>
       </c>
@@ -29893,6 +30934,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T129" t="n">
+        <v/>
+      </c>
+      <c r="U129" t="n">
+        <v/>
+      </c>
+      <c r="V129" t="n">
+        <v/>
+      </c>
+      <c r="W129" t="n">
+        <v/>
+      </c>
       <c r="X129" t="n">
         <v>2</v>
       </c>
@@ -29910,6 +30963,9 @@
       </c>
       <c r="AC129" t="n">
         <v>1</v>
+      </c>
+      <c r="AD129" t="n">
+        <v/>
       </c>
       <c r="AE129" t="n">
         <v>0</v>
@@ -29984,6 +31040,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H130" t="n">
+        <v/>
+      </c>
       <c r="I130" t="n">
         <v>90</v>
       </c>
@@ -30028,6 +31087,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U130" t="n">
+        <v/>
+      </c>
+      <c r="V130" t="n">
+        <v/>
+      </c>
+      <c r="W130" t="n">
+        <v/>
+      </c>
       <c r="X130" t="n">
         <v>2</v>
       </c>
@@ -30124,6 +31192,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H131" t="n">
+        <v/>
+      </c>
       <c r="I131" t="n">
         <v>90</v>
       </c>
@@ -30273,6 +31344,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H132" t="n">
+        <v/>
+      </c>
       <c r="I132" t="n">
         <v>90</v>
       </c>
@@ -30422,6 +31496,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H133" t="n">
+        <v/>
+      </c>
       <c r="I133" t="n">
         <v>90</v>
       </c>
@@ -30571,6 +31648,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H134" t="n">
+        <v/>
+      </c>
       <c r="I134" t="n">
         <v>90</v>
       </c>
@@ -30720,6 +31800,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H135" t="n">
+        <v/>
+      </c>
       <c r="I135" t="n">
         <v>90</v>
       </c>
@@ -30764,6 +31847,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U135" t="n">
+        <v/>
+      </c>
+      <c r="V135" t="n">
+        <v/>
+      </c>
+      <c r="W135" t="n">
+        <v/>
+      </c>
       <c r="X135" t="n">
         <v>2</v>
       </c>
@@ -30860,6 +31952,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H136" t="n">
+        <v/>
+      </c>
       <c r="I136" t="n">
         <v>90</v>
       </c>
@@ -30904,6 +31999,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U136" t="n">
+        <v/>
+      </c>
+      <c r="V136" t="n">
+        <v/>
+      </c>
+      <c r="W136" t="n">
+        <v/>
+      </c>
       <c r="X136" t="n">
         <v>2</v>
       </c>
@@ -31000,6 +32104,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H137" t="n">
+        <v/>
+      </c>
       <c r="I137" t="n">
         <v>90</v>
       </c>
@@ -31044,6 +32151,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U137" t="n">
+        <v/>
+      </c>
+      <c r="V137" t="n">
+        <v/>
+      </c>
+      <c r="W137" t="n">
+        <v/>
+      </c>
       <c r="X137" t="n">
         <v>2</v>
       </c>
@@ -31061,6 +32177,9 @@
       </c>
       <c r="AC137" t="n">
         <v>1</v>
+      </c>
+      <c r="AD137" t="n">
+        <v/>
       </c>
       <c r="AE137" t="n">
         <v>0</v>
@@ -31135,6 +32254,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H138" t="n">
+        <v/>
+      </c>
       <c r="I138" t="n">
         <v>90</v>
       </c>
@@ -31284,6 +32406,9 @@
           <t>MC2DNA-014</t>
         </is>
       </c>
+      <c r="H139" t="n">
+        <v/>
+      </c>
       <c r="I139" t="n">
         <v>150</v>
       </c>
@@ -31328,6 +32453,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U139" t="n">
+        <v/>
+      </c>
+      <c r="V139" t="n">
+        <v/>
+      </c>
+      <c r="W139" t="n">
+        <v/>
+      </c>
       <c r="X139" t="n">
         <v>2</v>
       </c>
@@ -31424,6 +32558,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H140" t="n">
+        <v/>
+      </c>
       <c r="I140" t="n">
         <v>90</v>
       </c>
@@ -31573,6 +32710,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H141" t="n">
+        <v/>
+      </c>
       <c r="I141" t="n">
         <v>20</v>
       </c>
@@ -31722,6 +32862,9 @@
           <t>MC2MCB-009</t>
         </is>
       </c>
+      <c r="H142" t="n">
+        <v/>
+      </c>
       <c r="I142" t="n">
         <v>100</v>
       </c>
@@ -31871,6 +33014,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H143" t="n">
+        <v/>
+      </c>
       <c r="I143" t="n">
         <v>60</v>
       </c>
@@ -32174,6 +33320,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H145" t="n">
+        <v/>
+      </c>
       <c r="I145" t="n">
         <v>45</v>
       </c>
@@ -32318,6 +33467,12 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="G146" t="n">
+        <v/>
+      </c>
+      <c r="H146" t="n">
+        <v/>
+      </c>
       <c r="I146" t="n">
         <v>45</v>
       </c>
@@ -32462,6 +33617,12 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="G147" t="n">
+        <v/>
+      </c>
+      <c r="H147" t="n">
+        <v/>
+      </c>
       <c r="I147" t="n">
         <v>55</v>
       </c>
@@ -32606,6 +33767,12 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="G148" t="n">
+        <v/>
+      </c>
+      <c r="H148" t="n">
+        <v/>
+      </c>
       <c r="I148" t="n">
         <v>55</v>
       </c>
@@ -32755,6 +33922,9 @@
           <t>MC2MCB-HYG-024</t>
         </is>
       </c>
+      <c r="H149" t="n">
+        <v/>
+      </c>
       <c r="I149" t="n">
         <v>60</v>
       </c>
@@ -32904,6 +34074,9 @@
           <t>MC2MCB-HYG-025</t>
         </is>
       </c>
+      <c r="H150" t="n">
+        <v/>
+      </c>
       <c r="I150" t="n">
         <v>60</v>
       </c>
@@ -33048,6 +34221,12 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="G151" t="n">
+        <v/>
+      </c>
+      <c r="H151" t="n">
+        <v/>
+      </c>
       <c r="I151" t="n">
         <v>40</v>
       </c>
@@ -33197,6 +34376,9 @@
           <t>MC2MCB-JLG-018</t>
         </is>
       </c>
+      <c r="H152" t="n">
+        <v/>
+      </c>
       <c r="I152" t="n">
         <v>65</v>
       </c>
@@ -33346,6 +34528,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H153" t="n">
+        <v/>
+      </c>
       <c r="I153" t="n">
         <v>40</v>
       </c>
@@ -33495,6 +34680,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H154" t="n">
+        <v/>
+      </c>
       <c r="I154" t="n">
         <v>65</v>
       </c>
@@ -33644,6 +34832,9 @@
           <t>MC2MCB-JLG-021</t>
         </is>
       </c>
+      <c r="H155" t="n">
+        <v/>
+      </c>
       <c r="I155" t="n">
         <v>40</v>
       </c>
@@ -33683,6 +34874,18 @@
           <t>SP2MCB-JLG-021</t>
         </is>
       </c>
+      <c r="T155" t="n">
+        <v/>
+      </c>
+      <c r="U155" t="n">
+        <v/>
+      </c>
+      <c r="V155" t="n">
+        <v/>
+      </c>
+      <c r="W155" t="n">
+        <v/>
+      </c>
       <c r="X155" t="n">
         <v>2</v>
       </c>
@@ -33700,6 +34903,9 @@
       </c>
       <c r="AC155" t="n">
         <v>0</v>
+      </c>
+      <c r="AD155" t="n">
+        <v/>
       </c>
       <c r="AE155" t="n">
         <v>0</v>
@@ -33774,6 +34980,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H156" t="n">
+        <v/>
+      </c>
       <c r="I156" t="n">
         <v>40</v>
       </c>
@@ -33916,6 +35125,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="G157" t="n">
+        <v/>
+      </c>
       <c r="H157" t="inlineStr">
         <is>
           <t>MC3-ASA-001</t>
@@ -34065,6 +35277,9 @@
           <t>MC3AW-015-V</t>
         </is>
       </c>
+      <c r="G158" t="n">
+        <v/>
+      </c>
       <c r="H158" t="inlineStr">
         <is>
           <t>MC3AW-015-V</t>
@@ -34113,6 +35328,15 @@
         <is>
           <t>SP3AW-015-V</t>
         </is>
+      </c>
+      <c r="U158" t="n">
+        <v/>
+      </c>
+      <c r="V158" t="n">
+        <v/>
+      </c>
+      <c r="W158" t="n">
+        <v/>
       </c>
       <c r="X158" t="n">
         <v>2</v>
@@ -34610,6 +35834,9 @@
           <t>Kulgachia - Small Line</t>
         </is>
       </c>
+      <c r="AH161" t="n">
+        <v/>
+      </c>
       <c r="AI161" t="n">
         <v>10</v>
       </c>
@@ -34759,6 +35986,9 @@
           <t>Kulgachia - Small Line</t>
         </is>
       </c>
+      <c r="AH162" t="n">
+        <v/>
+      </c>
       <c r="AI162" t="n">
         <v>12</v>
       </c>
@@ -34865,6 +36095,15 @@
           <t>SP3MGB-009-2T-NEO</t>
         </is>
       </c>
+      <c r="U163" t="n">
+        <v/>
+      </c>
+      <c r="V163" t="n">
+        <v/>
+      </c>
+      <c r="W163" t="n">
+        <v/>
+      </c>
       <c r="X163" t="n">
         <v>2</v>
       </c>
@@ -34899,6 +36138,9 @@
           <t>Kulgachia - Small Line</t>
         </is>
       </c>
+      <c r="AH163" t="n">
+        <v/>
+      </c>
       <c r="AI163" t="n">
         <v>12</v>
       </c>
@@ -34956,6 +36198,9 @@
           <t>KVCAD30MC001</t>
         </is>
       </c>
+      <c r="H164" t="n">
+        <v/>
+      </c>
       <c r="I164" t="n">
         <v>90</v>
       </c>
@@ -34995,6 +36240,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T164" t="n">
+        <v/>
+      </c>
+      <c r="U164" t="n">
+        <v/>
+      </c>
+      <c r="V164" t="n">
+        <v/>
+      </c>
+      <c r="W164" t="n">
+        <v/>
+      </c>
       <c r="X164" t="n">
         <v>2</v>
       </c>
@@ -35091,6 +36348,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H165" t="n">
+        <v/>
+      </c>
       <c r="I165" t="n">
         <v>40</v>
       </c>
@@ -35240,6 +36500,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H166" t="n">
+        <v/>
+      </c>
       <c r="I166" t="n">
         <v>40</v>
       </c>
@@ -35381,7 +36644,7 @@
       </c>
       <c r="F167" t="inlineStr">
         <is>
-          <t>BVCAD30MC001</t>
+          <t>KVCAD30MC001</t>
         </is>
       </c>
       <c r="G167" t="inlineStr">
@@ -35391,7 +36654,7 @@
       </c>
       <c r="H167" t="inlineStr">
         <is>
-          <t>BVCAD30MC001</t>
+          <t>KVCAD30MC001</t>
         </is>
       </c>
       <c r="I167" t="n">
@@ -35535,7 +36798,7 @@
       </c>
       <c r="F168" t="inlineStr">
         <is>
-          <t>BVCAD30MC001</t>
+          <t>KVCAD30MC001</t>
         </is>
       </c>
       <c r="G168" t="inlineStr">
@@ -35545,7 +36808,7 @@
       </c>
       <c r="H168" t="inlineStr">
         <is>
-          <t>BVCAD30MC001</t>
+          <t>KVCAD30MC001</t>
         </is>
       </c>
       <c r="I168" t="n">
@@ -35689,7 +36952,7 @@
       </c>
       <c r="F169" t="inlineStr">
         <is>
-          <t>BVCAD30MC001</t>
+          <t>KVCAD30MC001</t>
         </is>
       </c>
       <c r="G169" t="inlineStr">
@@ -35699,7 +36962,7 @@
       </c>
       <c r="H169" t="inlineStr">
         <is>
-          <t>BVCAD30MC001</t>
+          <t>KVCAD30MC001</t>
         </is>
       </c>
       <c r="I169" t="n">
@@ -35843,7 +37106,7 @@
       </c>
       <c r="F170" t="inlineStr">
         <is>
-          <t>BVCAD30MC001</t>
+          <t>KVCAD30MC001</t>
         </is>
       </c>
       <c r="G170" t="inlineStr">
@@ -35853,7 +37116,7 @@
       </c>
       <c r="H170" t="inlineStr">
         <is>
-          <t>BVCAD30MC001</t>
+          <t>KVCAD30MC001</t>
         </is>
       </c>
       <c r="I170" t="n">
@@ -36000,6 +37263,12 @@
           <t>MC-LKK-024</t>
         </is>
       </c>
+      <c r="G171" t="n">
+        <v/>
+      </c>
+      <c r="H171" t="n">
+        <v/>
+      </c>
       <c r="I171" t="n">
         <v>170</v>
       </c>
@@ -36039,6 +37308,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T171" t="n">
+        <v/>
+      </c>
+      <c r="U171" t="n">
+        <v/>
+      </c>
+      <c r="V171" t="n">
+        <v/>
+      </c>
+      <c r="W171" t="n">
+        <v/>
+      </c>
       <c r="X171" t="n">
         <v>2</v>
       </c>
@@ -36056,6 +37337,9 @@
       </c>
       <c r="AC171" t="n">
         <v>1</v>
+      </c>
+      <c r="AD171" t="n">
+        <v/>
       </c>
       <c r="AE171" t="n">
         <v>0</v>
@@ -36125,6 +37409,12 @@
           <t>MC-LKK-025</t>
         </is>
       </c>
+      <c r="G172" t="n">
+        <v/>
+      </c>
+      <c r="H172" t="n">
+        <v/>
+      </c>
       <c r="I172" t="n">
         <v>170</v>
       </c>
@@ -36164,6 +37454,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T172" t="n">
+        <v/>
+      </c>
+      <c r="U172" t="n">
+        <v/>
+      </c>
+      <c r="V172" t="n">
+        <v/>
+      </c>
+      <c r="W172" t="n">
+        <v/>
+      </c>
       <c r="X172" t="n">
         <v>2</v>
       </c>
@@ -36181,6 +37483,9 @@
       </c>
       <c r="AC172" t="n">
         <v>1</v>
+      </c>
+      <c r="AD172" t="n">
+        <v/>
       </c>
       <c r="AE172" t="n">
         <v>0</v>
@@ -36250,6 +37555,12 @@
           <t>MC-LKK-026</t>
         </is>
       </c>
+      <c r="G173" t="n">
+        <v/>
+      </c>
+      <c r="H173" t="n">
+        <v/>
+      </c>
       <c r="I173" t="n">
         <v>170</v>
       </c>
@@ -36289,6 +37600,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T173" t="n">
+        <v/>
+      </c>
+      <c r="U173" t="n">
+        <v/>
+      </c>
+      <c r="V173" t="n">
+        <v/>
+      </c>
+      <c r="W173" t="n">
+        <v/>
+      </c>
       <c r="X173" t="n">
         <v>2</v>
       </c>
@@ -36380,6 +37703,12 @@
           <t>MC-LKK-027</t>
         </is>
       </c>
+      <c r="G174" t="n">
+        <v/>
+      </c>
+      <c r="H174" t="n">
+        <v/>
+      </c>
       <c r="I174" t="n">
         <v>170</v>
       </c>
@@ -36419,6 +37748,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T174" t="n">
+        <v/>
+      </c>
+      <c r="U174" t="n">
+        <v/>
+      </c>
+      <c r="V174" t="n">
+        <v/>
+      </c>
+      <c r="W174" t="n">
+        <v/>
+      </c>
       <c r="X174" t="n">
         <v>2</v>
       </c>
@@ -36510,6 +37851,12 @@
           <t>MC-LKK-028</t>
         </is>
       </c>
+      <c r="G175" t="n">
+        <v/>
+      </c>
+      <c r="H175" t="n">
+        <v/>
+      </c>
       <c r="I175" t="n">
         <v>170</v>
       </c>
@@ -36549,6 +37896,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T175" t="n">
+        <v/>
+      </c>
+      <c r="U175" t="n">
+        <v/>
+      </c>
+      <c r="V175" t="n">
+        <v/>
+      </c>
+      <c r="W175" t="n">
+        <v/>
+      </c>
       <c r="X175" t="n">
         <v>2</v>
       </c>
@@ -36640,6 +37999,12 @@
           <t>MC-LKK-029</t>
         </is>
       </c>
+      <c r="G176" t="n">
+        <v/>
+      </c>
+      <c r="H176" t="n">
+        <v/>
+      </c>
       <c r="I176" t="n">
         <v>170</v>
       </c>
@@ -36679,6 +38044,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T176" t="n">
+        <v/>
+      </c>
+      <c r="U176" t="n">
+        <v/>
+      </c>
+      <c r="V176" t="n">
+        <v/>
+      </c>
+      <c r="W176" t="n">
+        <v/>
+      </c>
       <c r="X176" t="n">
         <v>2</v>
       </c>
@@ -37083,6 +38460,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H179" t="n">
+        <v/>
+      </c>
       <c r="I179" t="n">
         <v>40</v>
       </c>
@@ -37232,6 +38612,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H180" t="n">
+        <v/>
+      </c>
       <c r="I180" t="n">
         <v>40</v>
       </c>
@@ -37381,6 +38764,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H181" t="n">
+        <v/>
+      </c>
       <c r="I181" t="n">
         <v>40</v>
       </c>
@@ -37530,6 +38916,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H182" t="n">
+        <v/>
+      </c>
       <c r="I182" t="n">
         <v>40</v>
       </c>
@@ -37679,6 +39068,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H183" t="n">
+        <v/>
+      </c>
       <c r="I183" t="n">
         <v>40</v>
       </c>
@@ -37828,6 +39220,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H184" t="n">
+        <v/>
+      </c>
       <c r="I184" t="n">
         <v>40</v>
       </c>
@@ -37867,6 +39262,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T184" t="n">
+        <v/>
+      </c>
+      <c r="U184" t="n">
+        <v/>
+      </c>
+      <c r="V184" t="n">
+        <v/>
+      </c>
+      <c r="W184" t="n">
+        <v/>
+      </c>
       <c r="X184" t="n">
         <v>2</v>
       </c>
@@ -37884,6 +39291,9 @@
       </c>
       <c r="AC184" t="n">
         <v>1</v>
+      </c>
+      <c r="AD184" t="n">
+        <v/>
       </c>
       <c r="AE184" t="n">
         <v>0</v>
@@ -37958,6 +39368,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H185" t="n">
+        <v/>
+      </c>
       <c r="I185" t="n">
         <v>80</v>
       </c>
@@ -37997,6 +39410,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T185" t="n">
+        <v/>
+      </c>
+      <c r="U185" t="n">
+        <v/>
+      </c>
+      <c r="V185" t="n">
+        <v/>
+      </c>
+      <c r="W185" t="n">
+        <v/>
+      </c>
       <c r="X185" t="n">
         <v>2</v>
       </c>
@@ -38093,6 +39518,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H186" t="n">
+        <v/>
+      </c>
       <c r="I186" t="n">
         <v>80</v>
       </c>
@@ -38132,6 +39560,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T186" t="n">
+        <v/>
+      </c>
+      <c r="U186" t="n">
+        <v/>
+      </c>
+      <c r="V186" t="n">
+        <v/>
+      </c>
+      <c r="W186" t="n">
+        <v/>
+      </c>
       <c r="X186" t="n">
         <v>2</v>
       </c>
@@ -38149,6 +39589,9 @@
       </c>
       <c r="AC186" t="n">
         <v>1</v>
+      </c>
+      <c r="AD186" t="n">
+        <v/>
       </c>
       <c r="AE186" t="n">
         <v>0</v>
@@ -38223,6 +39666,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H187" t="n">
+        <v/>
+      </c>
       <c r="I187" t="n">
         <v>80</v>
       </c>
@@ -38262,6 +39708,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T187" t="n">
+        <v/>
+      </c>
+      <c r="U187" t="n">
+        <v/>
+      </c>
+      <c r="V187" t="n">
+        <v/>
+      </c>
+      <c r="W187" t="n">
+        <v/>
+      </c>
       <c r="X187" t="n">
         <v>2</v>
       </c>
@@ -38358,6 +39816,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H188" t="n">
+        <v/>
+      </c>
       <c r="I188" t="n">
         <v>40</v>
       </c>
@@ -38507,6 +39968,9 @@
           <t>KVCAD30MC001</t>
         </is>
       </c>
+      <c r="H189" t="n">
+        <v/>
+      </c>
       <c r="I189" t="n">
         <v>40</v>
       </c>
@@ -38546,6 +40010,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T189" t="n">
+        <v/>
+      </c>
+      <c r="U189" t="n">
+        <v/>
+      </c>
+      <c r="V189" t="n">
+        <v/>
+      </c>
+      <c r="W189" t="n">
+        <v/>
+      </c>
       <c r="X189" t="n">
         <v>2</v>
       </c>
@@ -38642,6 +40118,9 @@
           <t>KVCAD30MC001</t>
         </is>
       </c>
+      <c r="H190" t="n">
+        <v/>
+      </c>
       <c r="I190" t="n">
         <v>40</v>
       </c>
@@ -38681,6 +40160,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T190" t="n">
+        <v/>
+      </c>
+      <c r="U190" t="n">
+        <v/>
+      </c>
+      <c r="V190" t="n">
+        <v/>
+      </c>
+      <c r="W190" t="n">
+        <v/>
+      </c>
       <c r="X190" t="n">
         <v>2</v>
       </c>
@@ -38777,6 +40268,9 @@
           <t>KVCAD30MC001</t>
         </is>
       </c>
+      <c r="H191" t="n">
+        <v/>
+      </c>
       <c r="I191" t="n">
         <v>40</v>
       </c>
@@ -38816,6 +40310,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T191" t="n">
+        <v/>
+      </c>
+      <c r="U191" t="n">
+        <v/>
+      </c>
+      <c r="V191" t="n">
+        <v/>
+      </c>
+      <c r="W191" t="n">
+        <v/>
+      </c>
       <c r="X191" t="n">
         <v>2</v>
       </c>
@@ -38912,6 +40418,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H192" t="n">
+        <v/>
+      </c>
       <c r="I192" t="n">
         <v>40</v>
       </c>
@@ -38956,6 +40465,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U192" t="n">
+        <v/>
+      </c>
+      <c r="V192" t="n">
+        <v/>
+      </c>
+      <c r="W192" t="n">
+        <v/>
+      </c>
       <c r="X192" t="n">
         <v>2</v>
       </c>
@@ -39052,6 +40570,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H193" t="n">
+        <v/>
+      </c>
       <c r="I193" t="n">
         <v>40</v>
       </c>
@@ -39096,6 +40617,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U193" t="n">
+        <v/>
+      </c>
+      <c r="V193" t="n">
+        <v/>
+      </c>
+      <c r="W193" t="n">
+        <v/>
+      </c>
       <c r="X193" t="n">
         <v>2</v>
       </c>
@@ -39189,8 +40719,11 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>BVCAD50MC001</t>
-        </is>
+          <t>KVCAD50MC001</t>
+        </is>
+      </c>
+      <c r="H194" t="n">
+        <v/>
       </c>
       <c r="I194" t="n">
         <v>40</v>
@@ -39231,6 +40764,18 @@
           <t>BVCALPPSP002</t>
         </is>
       </c>
+      <c r="T194" t="n">
+        <v/>
+      </c>
+      <c r="U194" t="n">
+        <v/>
+      </c>
+      <c r="V194" t="n">
+        <v/>
+      </c>
+      <c r="W194" t="n">
+        <v/>
+      </c>
       <c r="X194" t="n">
         <v>2</v>
       </c>
@@ -39327,6 +40872,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H195" t="n">
+        <v/>
+      </c>
       <c r="I195" t="n">
         <v>40</v>
       </c>
@@ -39366,6 +40914,18 @@
           <t>KVCALPPSP002</t>
         </is>
       </c>
+      <c r="T195" t="n">
+        <v/>
+      </c>
+      <c r="U195" t="n">
+        <v/>
+      </c>
+      <c r="V195" t="n">
+        <v/>
+      </c>
+      <c r="W195" t="n">
+        <v/>
+      </c>
       <c r="X195" t="n">
         <v>2</v>
       </c>
@@ -39457,6 +41017,12 @@
           <t>MC-UBC-053</t>
         </is>
       </c>
+      <c r="G196" t="n">
+        <v/>
+      </c>
+      <c r="H196" t="n">
+        <v/>
+      </c>
       <c r="I196" t="n">
         <v>50</v>
       </c>
@@ -39501,6 +41067,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U196" t="n">
+        <v/>
+      </c>
+      <c r="V196" t="n">
+        <v/>
+      </c>
+      <c r="W196" t="n">
+        <v/>
+      </c>
       <c r="X196" t="n">
         <v>2</v>
       </c>
@@ -39597,6 +41172,9 @@
           <t>KVCAD30MC001</t>
         </is>
       </c>
+      <c r="H197" t="n">
+        <v/>
+      </c>
       <c r="I197" t="n">
         <v>90</v>
       </c>
@@ -39636,6 +41214,18 @@
           <t>BVCALPPSP002</t>
         </is>
       </c>
+      <c r="T197" t="n">
+        <v/>
+      </c>
+      <c r="U197" t="n">
+        <v/>
+      </c>
+      <c r="V197" t="n">
+        <v/>
+      </c>
+      <c r="W197" t="n">
+        <v/>
+      </c>
       <c r="X197" t="n">
         <v>2</v>
       </c>
@@ -39732,6 +41322,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H198" t="n">
+        <v/>
+      </c>
       <c r="I198" t="n">
         <v>90</v>
       </c>
@@ -39776,6 +41369,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U198" t="n">
+        <v/>
+      </c>
+      <c r="V198" t="n">
+        <v/>
+      </c>
+      <c r="W198" t="n">
+        <v/>
+      </c>
       <c r="X198" t="n">
         <v>2</v>
       </c>
@@ -39793,6 +41395,9 @@
       </c>
       <c r="AC198" t="n">
         <v>1</v>
+      </c>
+      <c r="AD198" t="n">
+        <v/>
       </c>
       <c r="AE198" t="n">
         <v>0</v>
@@ -39867,6 +41472,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H199" t="n">
+        <v/>
+      </c>
       <c r="I199" t="n">
         <v>90</v>
       </c>
@@ -39911,6 +41519,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U199" t="n">
+        <v/>
+      </c>
+      <c r="V199" t="n">
+        <v/>
+      </c>
+      <c r="W199" t="n">
+        <v/>
+      </c>
       <c r="X199" t="n">
         <v>2</v>
       </c>
@@ -39928,6 +41545,9 @@
       </c>
       <c r="AC199" t="n">
         <v>1</v>
+      </c>
+      <c r="AD199" t="n">
+        <v/>
       </c>
       <c r="AE199" t="n">
         <v>0</v>
@@ -40002,6 +41622,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H200" t="n">
+        <v/>
+      </c>
       <c r="I200" t="n">
         <v>40</v>
       </c>
@@ -40046,6 +41669,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U200" t="n">
+        <v/>
+      </c>
+      <c r="V200" t="n">
+        <v/>
+      </c>
+      <c r="W200" t="n">
+        <v/>
+      </c>
       <c r="X200" t="n">
         <v>2</v>
       </c>
@@ -40063,6 +41695,9 @@
       </c>
       <c r="AC200" t="n">
         <v>1</v>
+      </c>
+      <c r="AD200" t="n">
+        <v/>
       </c>
       <c r="AE200" t="n">
         <v>0</v>
@@ -40137,6 +41772,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H201" t="n">
+        <v/>
+      </c>
       <c r="I201" t="n">
         <v>40</v>
       </c>
@@ -40181,6 +41819,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U201" t="n">
+        <v/>
+      </c>
+      <c r="V201" t="n">
+        <v/>
+      </c>
+      <c r="W201" t="n">
+        <v/>
+      </c>
       <c r="X201" t="n">
         <v>2</v>
       </c>
@@ -40198,6 +41845,9 @@
       </c>
       <c r="AC201" t="n">
         <v>1</v>
+      </c>
+      <c r="AD201" t="n">
+        <v/>
       </c>
       <c r="AE201" t="n">
         <v>0</v>
@@ -40272,6 +41922,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H202" t="n">
+        <v/>
+      </c>
       <c r="I202" t="n">
         <v>40</v>
       </c>
@@ -40316,6 +41969,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U202" t="n">
+        <v/>
+      </c>
+      <c r="V202" t="n">
+        <v/>
+      </c>
+      <c r="W202" t="n">
+        <v/>
+      </c>
       <c r="X202" t="n">
         <v>2</v>
       </c>
@@ -40333,6 +41995,9 @@
       </c>
       <c r="AC202" t="n">
         <v>1</v>
+      </c>
+      <c r="AD202" t="n">
+        <v/>
       </c>
       <c r="AE202" t="n">
         <v>0</v>
@@ -40405,6 +42070,9 @@
           <t>KVCAD50MC001</t>
         </is>
       </c>
+      <c r="H203" t="n">
+        <v/>
+      </c>
       <c r="I203" t="n">
         <v>40</v>
       </c>
@@ -40449,6 +42117,15 @@
           <t>KVCALFPSP001</t>
         </is>
       </c>
+      <c r="U203" t="n">
+        <v/>
+      </c>
+      <c r="V203" t="n">
+        <v/>
+      </c>
+      <c r="W203" t="n">
+        <v/>
+      </c>
       <c r="X203" t="n">
         <v>2</v>
       </c>
@@ -40466,6 +42143,9 @@
       </c>
       <c r="AC203" t="n">
         <v>1</v>
+      </c>
+      <c r="AD203" t="n">
+        <v/>
       </c>
       <c r="AE203" t="n">
         <v>0</v>
@@ -40533,6 +42213,12 @@
           <t>MC1-KBS-014</t>
         </is>
       </c>
+      <c r="G204" t="n">
+        <v/>
+      </c>
+      <c r="H204" t="n">
+        <v/>
+      </c>
       <c r="I204" t="n">
         <v>20</v>
       </c>
@@ -40567,6 +42253,21 @@
           <t>SP1-KBS-014</t>
         </is>
       </c>
+      <c r="S204" t="n">
+        <v/>
+      </c>
+      <c r="T204" t="n">
+        <v/>
+      </c>
+      <c r="U204" t="n">
+        <v/>
+      </c>
+      <c r="V204" t="n">
+        <v/>
+      </c>
+      <c r="W204" t="n">
+        <v/>
+      </c>
       <c r="X204" t="n">
         <v>2</v>
       </c>
@@ -40584,6 +42285,9 @@
       </c>
       <c r="AC204" t="n">
         <v>0</v>
+      </c>
+      <c r="AD204" t="n">
+        <v/>
       </c>
       <c r="AE204" t="n">
         <v>0</v>

</xml_diff>